<commit_message>
fix : StoreCertification도 Database에서 데이터 중복이 일어나지 않도록 수정 (#19)
</commit_message>
<xml_diff>
--- a/src/main/resources/data/mobeom/mobeom_test.xlsx
+++ b/src/main/resources/data/mobeom/mobeom_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/logan/Desktop/Logan/project/Spring/nainga/src/main/resources/data/mobeom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A172AC5D-A01D-FD4E-AECA-16861FC210B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05FDE3E-4D54-C54B-AB89-E4E2633E902F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -695,7 +695,7 @@
   <dimension ref="A1:X6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
-      <selection activeCell="H29" sqref="H29"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
feat : GoogleMapStoreService 내 모든 로직에 대한 테스트 코드 작성 (#19)
</commit_message>
<xml_diff>
--- a/src/main/resources/data/mobeom/mobeom_test.xlsx
+++ b/src/main/resources/data/mobeom/mobeom_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/logan/Desktop/Logan/project/Spring/nainga/src/main/resources/data/mobeom/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F05FDE3E-4D54-C54B-AB89-E4E2633E902F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C719A30F-370E-8E40-A9AC-16617B61CF15}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19580" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="94">
   <si>
     <t>번호</t>
   </si>
@@ -692,10 +692,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:X6"/>
+  <dimension ref="A1:X7"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="105" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1145,6 +1145,77 @@
         <v>93</v>
       </c>
     </row>
+    <row r="7" spans="1:24" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>83</v>
+      </c>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" t="s">
+        <v>84</v>
+      </c>
+      <c r="E7" t="s">
+        <v>85</v>
+      </c>
+      <c r="F7" t="s">
+        <v>86</v>
+      </c>
+      <c r="G7" t="s">
+        <v>87</v>
+      </c>
+      <c r="H7" t="s">
+        <v>88</v>
+      </c>
+      <c r="I7" t="s">
+        <v>62</v>
+      </c>
+      <c r="J7" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" t="s">
+        <v>30</v>
+      </c>
+      <c r="L7" t="s">
+        <v>89</v>
+      </c>
+      <c r="M7" t="s">
+        <v>36</v>
+      </c>
+      <c r="O7" t="s">
+        <v>30</v>
+      </c>
+      <c r="P7" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" t="s">
+        <v>30</v>
+      </c>
+      <c r="R7" t="s">
+        <v>90</v>
+      </c>
+      <c r="S7" t="s">
+        <v>91</v>
+      </c>
+      <c r="T7" t="s">
+        <v>68</v>
+      </c>
+      <c r="U7" t="s">
+        <v>92</v>
+      </c>
+      <c r="V7" t="s">
+        <v>70</v>
+      </c>
+      <c r="W7" t="s">
+        <v>71</v>
+      </c>
+      <c r="X7" t="s">
+        <v>93</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>